<commit_message>
updated tests, plotted test cells on excel spreadsheet
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="53">
   <si>
     <t>CL</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -210,6 +210,24 @@
   </si>
   <si>
     <t>Yellow: Door Dir test</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Orange : Adj In Room</t>
+  </si>
+  <si>
+    <t>Blue: Room Exit</t>
+  </si>
+  <si>
+    <t>Purple: Adj to door</t>
+  </si>
+  <si>
+    <t>Brown: Walkway adj</t>
+  </si>
+  <si>
+    <t>Grey: Door enter target</t>
   </si>
 </sst>
 </file>
@@ -234,7 +252,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +286,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -390,12 +450,38 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF33CC33"/>
+      <color rgb="FFFF99CC"/>
+      <color rgb="FFE08EBD"/>
+      <color rgb="FFE6888A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -730,7 +816,7 @@
   <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -753,10 +839,10 @@
       <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="36" t="s">
         <v>31</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -973,7 +1059,7 @@
       <c r="T3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="U3" s="30" t="s">
         <v>35</v>
       </c>
       <c r="V3" s="9" t="s">
@@ -1171,7 +1257,7 @@
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="37" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1290,7 +1376,7 @@
       <c r="K7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="34" t="s">
         <v>22</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -1376,7 +1462,7 @@
       <c r="K8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="L8" s="33" t="s">
         <v>35</v>
       </c>
       <c r="M8" s="8" t="s">
@@ -1507,7 +1593,7 @@
       <c r="Z9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AA9" s="11" t="s">
+      <c r="AA9" s="39" t="s">
         <v>35</v>
       </c>
       <c r="AB9" s="20">
@@ -1533,7 +1619,7 @@
       <c r="F10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="29" t="s">
         <v>43</v>
       </c>
       <c r="H10" s="8" t="s">
@@ -1560,7 +1646,7 @@
       <c r="O10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="32" t="s">
         <v>35</v>
       </c>
       <c r="Q10" s="8" t="s">
@@ -1578,7 +1664,7 @@
       <c r="U10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="V10" s="7" t="s">
+      <c r="V10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="W10" s="6" t="s">
@@ -1741,7 +1827,7 @@
       <c r="R12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="S12" s="27" t="s">
         <v>35</v>
       </c>
       <c r="T12" s="8" t="s">
@@ -1788,7 +1874,7 @@
       <c r="E13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="30" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="8" t="s">
@@ -1815,7 +1901,7 @@
       <c r="N13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="O13" s="27" t="s">
         <v>35</v>
       </c>
       <c r="P13" s="8" t="s">
@@ -1862,7 +1948,7 @@
       <c r="A14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="40" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1963,7 +2049,7 @@
       <c r="F15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="32" t="s">
         <v>35</v>
       </c>
       <c r="H15" s="8" t="s">
@@ -2049,7 +2135,7 @@
       <c r="F16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="33" t="s">
         <v>35</v>
       </c>
       <c r="H16" s="8" t="s">
@@ -2094,7 +2180,7 @@
       <c r="U16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="V16" s="8" t="s">
+      <c r="V16" s="32" t="s">
         <v>35</v>
       </c>
       <c r="W16" s="8" t="s">
@@ -2147,7 +2233,7 @@
       <c r="J17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="33" t="s">
         <v>35</v>
       </c>
       <c r="L17" s="8" t="s">
@@ -2227,7 +2313,7 @@
       <c r="H18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="29" t="s">
         <v>6</v>
       </c>
       <c r="J18" s="6" t="s">
@@ -2254,10 +2340,10 @@
       <c r="Q18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R18" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="S18" s="8" t="s">
+      <c r="R18" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="S18" s="40" t="s">
         <v>35</v>
       </c>
       <c r="T18" s="8" t="s">
@@ -2358,7 +2444,7 @@
       <c r="W19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="X19" s="8" t="s">
+      <c r="X19" s="30" t="s">
         <v>35</v>
       </c>
       <c r="Y19" s="8" t="s">
@@ -2441,7 +2527,7 @@
       <c r="V20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="W20" s="7" t="s">
+      <c r="W20" s="29" t="s">
         <v>8</v>
       </c>
       <c r="X20" s="7" t="s">
@@ -2476,7 +2562,7 @@
       <c r="E21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="27" t="s">
         <v>35</v>
       </c>
       <c r="G21" s="6" t="s">
@@ -2506,8 +2592,8 @@
       <c r="O21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P21" s="6" t="s">
-        <v>25</v>
+      <c r="P21" s="27" t="s">
+        <v>47</v>
       </c>
       <c r="Q21" s="6" t="s">
         <v>25</v>
@@ -2675,7 +2761,7 @@
       <c r="N23" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="O23" s="16" t="s">
+      <c r="O23" s="38" t="s">
         <v>35</v>
       </c>
       <c r="P23" s="15" t="s">
@@ -2913,7 +2999,9 @@
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
+      <c r="O28" s="25" t="s">
+        <v>48</v>
+      </c>
       <c r="P28" s="18"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="18"/>
@@ -2944,7 +3032,9 @@
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
+      <c r="O29" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="P29" s="18"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="18"/>
@@ -2975,7 +3065,9 @@
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
+      <c r="O30" s="31" t="s">
+        <v>50</v>
+      </c>
       <c r="P30" s="18"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="18"/>
@@ -3006,7 +3098,9 @@
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
+      <c r="O31" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="P31" s="18"/>
       <c r="Q31" s="18"/>
       <c r="R31" s="18"/>
@@ -3037,7 +3131,9 @@
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
+      <c r="O32" s="41" t="s">
+        <v>52</v>
+      </c>
       <c r="P32" s="18"/>
       <c r="Q32" s="18"/>
       <c r="R32" s="18"/>

</xml_diff>